<commit_message>
second commit with fixed test
</commit_message>
<xml_diff>
--- a/Kopiec Binarny.xlsx
+++ b/Kopiec Binarny.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
   <si>
     <t>Dodawanie elementu</t>
   </si>
@@ -20,7 +20,7 @@
     <t>Ilosc opreacji</t>
   </si>
   <si>
-    <t>Czas [ms]</t>
+    <t>Czas []</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -81,14 +81,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="27.01953125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="9.45703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.83984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="27.01953125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -106,82 +108,82 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>50000.0</v>
+        <v>5000.0</v>
       </c>
       <c r="B3" t="n">
-        <v>8.0</v>
+        <v>323.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>100000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="B4" t="n">
-        <v>4.0</v>
+        <v>246.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>150000.0</v>
+        <v>15000.0</v>
       </c>
       <c r="B5" t="n">
-        <v>4.0</v>
+        <v>146.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>200000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="B6" t="n">
-        <v>5.0</v>
+        <v>86.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>250000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="B7" t="n">
-        <v>10.0</v>
+        <v>72.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>300000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="B8" t="n">
-        <v>11.0</v>
+        <v>71.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>350000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="B9" t="n">
-        <v>12.0</v>
+        <v>89.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>400000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="B10" t="n">
-        <v>15.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>450000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="B11" t="n">
-        <v>16.0</v>
+        <v>83.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>500000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="B12" t="n">
-        <v>17.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="13">
@@ -198,6 +200,15 @@
       <c r="A15" t="s">
         <v>4</v>
       </c>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -206,85 +217,175 @@
       <c r="B16" t="s">
         <v>2</v>
       </c>
+      <c r="E16" t="n">
+        <v>5000.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>323.0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>4345.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>50000.0</v>
+        <v>5000.0</v>
       </c>
       <c r="B17" t="n">
-        <v>406.0</v>
+        <v>4345.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>246.0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>4410.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>100000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="B18" t="n">
-        <v>3136.0</v>
+        <v>4410.0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>15000.0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>146.0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>6135.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>150000.0</v>
+        <v>15000.0</v>
       </c>
       <c r="B19" t="n">
-        <v>9833.0</v>
+        <v>6135.0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>86.0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9683.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>200000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="B20" t="n">
-        <v>23175.0</v>
+        <v>9683.0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>25000.0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>18508.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>250000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="B21" t="n">
-        <v>48831.0</v>
+        <v>18508.0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>21946.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>300000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="B22" t="n">
-        <v>82800.0</v>
+        <v>21946.0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>28419.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>350000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="B23" t="n">
-        <v>138199.0</v>
+        <v>28419.0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>33522.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>400000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="B24" t="n">
-        <v>190091.0</v>
+        <v>33522.0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>45000.0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>38631.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>450000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="B25" t="n">
-        <v>217544.0</v>
+        <v>38631.0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>50000.0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>41336.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>500000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="B26" t="n">
-        <v>266533.0</v>
+        <v>41336.0</v>
       </c>
     </row>
     <row r="27">
@@ -301,6 +402,15 @@
       <c r="A29" t="s">
         <v>5</v>
       </c>
+      <c r="E29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
@@ -309,85 +419,175 @@
       <c r="B30" t="s">
         <v>2</v>
       </c>
+      <c r="E30" t="n">
+        <v>5000.0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>4345.0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>180.0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>50000.0</v>
+        <v>5000.0</v>
       </c>
       <c r="B31" t="n">
-        <v>17.0</v>
+        <v>180.0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>10000.0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4410.0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>88.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>100000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="B32" t="n">
-        <v>3.0</v>
+        <v>88.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>15000.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>6135.0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>49.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>150000.0</v>
+        <v>15000.0</v>
       </c>
       <c r="B33" t="n">
-        <v>5.0</v>
+        <v>49.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>9683.0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>36.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>200000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="B34" t="n">
-        <v>24.0</v>
+        <v>36.0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>25000.0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>18508.0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>34.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>250000.0</v>
+        <v>25000.0</v>
       </c>
       <c r="B35" t="n">
-        <v>9.0</v>
+        <v>34.0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>30000.0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>21946.0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>35.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>300000.0</v>
+        <v>30000.0</v>
       </c>
       <c r="B36" t="n">
-        <v>13.0</v>
+        <v>35.0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>28419.0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>34.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>350000.0</v>
+        <v>35000.0</v>
       </c>
       <c r="B37" t="n">
         <v>34.0</v>
       </c>
+      <c r="E37" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>33522.0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>35.0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>400000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="B38" t="n">
-        <v>15.0</v>
+        <v>35.0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>45000.0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>38631.0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>34.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>450000.0</v>
+        <v>45000.0</v>
       </c>
       <c r="B39" t="n">
-        <v>25.0</v>
+        <v>34.0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>50000.0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>41336.0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>71.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>500000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="B40" t="n">
-        <v>18.0</v>
+        <v>71.0</v>
       </c>
     </row>
     <row r="41">

</xml_diff>